<commit_message>
Implementado multithreading para 2/4/6 nucleos en Mutex
</commit_message>
<xml_diff>
--- a/Concept-0/tasks.xlsx
+++ b/Concept-0/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bb54ded66f80c8e/UC3M/Cuarto Curso/Trabajo de Fin de Grado/Concept 0/Concept-0/Concept-0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_27B0EA2CD6B70B54146E1C4A26EB97FADFBBB3E8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{51A44EDA-F23D-4B7E-BF22-3C9BBB9800FE}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="11_27B0EA2CD6B70B54146E1C4A26EB97FADFBBB3E8" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38355E3B-DF7B-4790-B048-1B0ACF3206C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0">Tasks!$A$1:$C$26</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0">Tasks!$A$1:$C$30</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -145,13 +145,25 @@
   </si>
   <si>
     <t>Future Viability</t>
+  </si>
+  <si>
+    <t>Societary Type</t>
+  </si>
+  <si>
+    <t>Collective Agreement</t>
+  </si>
+  <si>
+    <t>Employees Salary</t>
+  </si>
+  <si>
+    <t>Investment Oportunities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -163,6 +175,12 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -221,8 +239,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Employees" displayName="Employees" ref="A1:D26" totalsRowShown="0">
-  <autoFilter ref="A1:D26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Employees" displayName="Employees" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Duration" dataDxfId="0"/>
@@ -530,15 +548,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.5546875" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
@@ -745,13 +763,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -765,15 +783,15 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B17" s="5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
@@ -785,27 +803,27 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="5">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B19" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -813,10 +831,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B20" s="5">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -827,27 +845,27 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B21" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B22" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -855,27 +873,27 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
         <v>29</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -883,13 +901,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -897,10 +915,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -909,7 +927,64 @@
         <v>4</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="5">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="5">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="5">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="5">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">

</xml_diff>